<commit_message>
Update : Inventory MVP패턴으로 현재 구현 중 및 ItemDB에 있는 Icon 경로 적용
</commit_message>
<xml_diff>
--- a/Assets/Resources/ExcelDB/ItemDB.xlsx
+++ b/Assets/Resources/ExcelDB/ItemDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONG\Desktop\개발\TIL\20241126\외부데이터로드\ExcelToJsonWizard.v1.0.6\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB75177-078E-4E44-AF0E-E27E6F46260E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F900BD-9EB9-47F1-9C62-7DE10E9B17A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66259E55-575D-4AFB-9E5A-BFDBC4B3828F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66259E55-575D-4AFB-9E5A-BFDBC4B3828F}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -88,85 +88,171 @@
     <t>bool</t>
   </si>
   <si>
-    <t>나무검</t>
+    <t>key</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconPath</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll2</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll3</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll4</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll5</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll6</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll7</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll8</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll9</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll10</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll11</t>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll12</t>
+  </si>
+  <si>
+    <t>연습용 공격 스크롤1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>연습용 공격 스크롤2</t>
+  </si>
+  <si>
+    <t>연습용 공격 스크롤3</t>
+  </si>
+  <si>
+    <t>연습용 공격 스크롤4</t>
+  </si>
+  <si>
+    <t>연습용 방어 스크롤1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>연습용 방어 스크롤2</t>
+  </si>
+  <si>
+    <t>연습용 방어 스크롤3</t>
+  </si>
+  <si>
+    <t>연습용 방어 스크롤4</t>
+  </si>
+  <si>
+    <t>연습용 치명 스크롤1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>연습용 치명 스크롤2</t>
+  </si>
+  <si>
+    <t>연습용 치명 스크롤3</t>
+  </si>
+  <si>
+    <t>연습용 치명 스크롤4</t>
+  </si>
+  <si>
+    <t>연습용 종합 스크롤1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Weapon</t>
-  </si>
-  <si>
-    <t>Common</t>
-  </si>
-  <si>
-    <t>평범한 나무 검이다.</t>
-  </si>
-  <si>
-    <t>없음</t>
-  </si>
-  <si>
-    <t>철검</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Rare</t>
-  </si>
-  <si>
-    <t>철로 만든 검이다.</t>
-  </si>
-  <si>
-    <t>황동검</t>
-  </si>
-  <si>
-    <t>황동으로 만든 검이다. 웬지 기분이 나쁘다.</t>
-  </si>
-  <si>
-    <t>은검</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격용 하급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격용 중급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격용 상급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격용 전설 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어용 하급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어용 중급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어용 상급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어용 전설 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>치명용 하급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>치명용 중급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>치명용 상급 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>치명용 전설 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 능력치를 올려주는 전설 스크롤이다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Epic</t>
-  </si>
-  <si>
-    <t>은으로 만든 검이다. 1인분은 하는것 같다.</t>
-  </si>
-  <si>
-    <t>금검</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Legendary</t>
-  </si>
-  <si>
-    <t>금으로 만든 검이다. 이제 좀 치는것 같다.</t>
-  </si>
-  <si>
-    <t>하급회복포션</t>
-  </si>
-  <si>
-    <t>Consummable</t>
-  </si>
-  <si>
-    <t>HP회복 포션이다. 30의 체력을 올려준다.</t>
-  </si>
-  <si>
-    <t>HP회복</t>
-  </si>
-  <si>
-    <t>중급회복포션</t>
-  </si>
-  <si>
-    <t>HP회복 포션이다. 50의 체력을 올려준다.</t>
-  </si>
-  <si>
-    <t>상급회복포션</t>
-  </si>
-  <si>
-    <t>HP회복 포션이다. 100의 체력을 올려준다.</t>
-  </si>
-  <si>
-    <t>엘릭서</t>
-  </si>
-  <si>
-    <t>HP회복 포션이다. 50% 체력을 올려준다.</t>
-  </si>
-  <si>
-    <t>key</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Item/Scroll/scroll13</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1151,17 +1237,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA74EC2-FB62-4265-9B64-B622478521B3}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1214,8 +1309,11 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1270,8 +1368,11 @@
       <c r="R2" t="s">
         <v>18</v>
       </c>
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1326,22 +1427,25 @@
       <c r="R3" t="s">
         <v>17</v>
       </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1000</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1362,45 +1466,45 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>26</v>
-      </c>
       <c r="Q4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="R4">
         <v>1</v>
       </c>
+      <c r="S4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -1418,19 +1522,16 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
       </c>
       <c r="Q5">
         <v>100</v>
@@ -1438,31 +1539,34 @@
       <c r="R5">
         <v>1</v>
       </c>
+      <c r="S5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1002</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
@@ -1474,51 +1578,51 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" t="b">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O6" t="b">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
-        <v>26</v>
-      </c>
       <c r="Q6">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
+      <c r="S6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1003</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -1530,305 +1634,529 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="b">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O7" t="b">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
-        <v>26</v>
-      </c>
       <c r="Q7">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="R7">
         <v>1</v>
       </c>
+      <c r="S7" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1004</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F8">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
       </c>
       <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <v>10</v>
       </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>5</v>
-      </c>
-      <c r="M8" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>150</v>
-      </c>
-      <c r="O8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q8">
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1005</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>100</v>
       </c>
-      <c r="R8">
-        <v>1</v>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2000</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1006</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>30</v>
       </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q9">
-        <v>200</v>
-      </c>
-      <c r="R9">
-        <v>999</v>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1000</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2001</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>50</v>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q10">
-        <v>200</v>
-      </c>
-      <c r="R10">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2002</v>
+        <v>1007</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>10000</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1008</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1009</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>30</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13">
         <v>100</v>
       </c>
-      <c r="K11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q11">
-        <v>200</v>
-      </c>
-      <c r="R11">
-        <v>999</v>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2003</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1010</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>30</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>50</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1000</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1011</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>50</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>10000</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>30</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q12">
-        <v>200</v>
-      </c>
-      <c r="R12">
-        <v>999</v>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1012</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>99999</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>